<commit_message>
Ajout d'une meta description pour index.html
</commit_message>
<xml_diff>
--- a/audit_seo.xlsx
+++ b/audit_seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -41,16 +41,71 @@
   </si>
   <si>
     <t xml:space="preserve">(SEO ou accessiblité ?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.2): langue de la page index.html paramétrée sur “default”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peut occasionner des difficultés de lectures pour les utilisateurs de lecteurs d’écran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paramétrer la langue en fonction de celle utilisée par la page (spécifier pour des passages qui seraient dans une autre langue si besoin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">régler la langue sur “fr”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.5): utilisation multiple du mot clé “agence design”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En plus de créer une répétition inutile, il est préférable d’éviter les pratiques pouvant être interprétées comme un abus de fonctionnement des algorithmes de recherche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choisir des mots clés pertinents en favorisant l’approche longue traîne à l’approche courte traîne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.5): utilisation du mot clé “agence design Paris” alors que l’agence est basée à Lyon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indiquer une autre localisation que celle de l’enseigne de l’agence induira les visiteurs potentiels en erreur leurs de leur recherche, en plus de créer une plus grande concurrence dans les résultats de recherche (Paris vs Lyon)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les mots clés locaux doivent désigner la même localisation que celle indiquée sur le site web et qui reflète la position géographique réelle de l’enseigne physique de l’agence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplacer “Paris” par “Lyon”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.6): meta “description” vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la meta description représente le texte qui sera affiché sous le titre et url du site dans les résultats de recherche, et est un facteur important d’attraction pour les visiteurs potentiels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utiliser une description pertinente (incluant les mots clés du site) et consise (moins de 140-160 caractères) tout en restant attirante pour les visiteurs potentiels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exemple de description : “La Chouette agence web design à Lyon : réalisez votre projet web grâce à notre expertise”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="[$$-2000]#,##0.00;[RED]\-[$$-2000]#,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -102,6 +157,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -151,25 +212,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -249,104 +322,162 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="21.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="1" width="11.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E3" s="4"/>
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E4" s="4"/>
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E5" s="4"/>
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E6" s="4"/>
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E8" s="4"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E9" s="4"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E10" s="4"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E11" s="4"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E12" s="4"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E13" s="4"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E14" s="4"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E15" s="4"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1334,6 +1465,9 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" display="https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Ajout d'un titre pour le site
</commit_message>
<xml_diff>
--- a/audit_seo.xlsx
+++ b/audit_seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">remplacer “Paris” par “Lyon”</t>
   </si>
   <si>
-    <t xml:space="preserve">(index.html l.6): meta “description” vide</t>
+    <t xml:space="preserve">(index.html l.6): meta description vide</t>
   </si>
   <si>
     <t xml:space="preserve">la meta description représente le texte qui sera affiché sous le titre et url du site dans les résultats de recherche, et est un facteur important d’attraction pour les visiteurs potentiels</t>
@@ -95,6 +95,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO/accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.22): meta title vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la meta titre est ce qui sera affiché en premier lors de l’apparition du site web dans les résultats de recherche et se doit donc d’être attractif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utiliser un titre concis et reprenant des mots clés de manière pertinente et naturelle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exemple de titre : “La Chouette agence | Experts web design à Lyon”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq</t>
   </si>
 </sst>
 </file>
@@ -325,7 +343,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -453,7 +471,24 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E7" s="5"/>
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E8" s="5"/>
@@ -1467,6 +1502,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" display="https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB"/>
+    <hyperlink ref="F7" r:id="rId2" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Modification description logo La Chouette + suppression balise vide <li></li>
</commit_message>
<xml_diff>
--- a/audit_seo.xlsx
+++ b/audit_seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -113,6 +113,51 @@
   </si>
   <si>
     <t xml:space="preserve">https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.40 et l.42): texte “caché” comprenant des mots clés pour tromper les algorithmes de Google lors de la lecture de la page web pour son référencement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ce genre de pratique, en plus d’être de mieux en mieux détecté par les algorithmes de Google, peut amener à une pénalisation du site web dans son référencement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n’utiliser des mots clés que dans des contextes pertinents et proscrire ce genre de pratique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer ces balises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.41): description subjective du site dans une balise alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les balises alt servent non seulement à décrire un élément visuel, mais sont également utilisées pour vérifier la pertinence d’un contenu par les moteurs de recherche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">se contenter d’utiliser les balises alt pour fournir de courtes descriptions objectives des éléments relatifs à celles-ci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exemple de description : “logo La Chouette agence”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">???SEO???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.52 et l.53): balise &lt;li&gt;&lt;/li&gt; vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.55): nom affiché sur le site pour la redirection vers page2.html (“page2 &amp;gt;”)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en plus de la faute de frappe pouvait donner une image amateure du site et le décrédibiliser auprès des visiteurs, nommer un lien “page2” ne permet pas de savoir vers quoi celui-ci redirige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les liens affichés sur le site devraient refléter clairement le type de contenu vers lequels ils redirigent afin de faciliter la navigation sur le site web, d’autant plus pour les personnes utilisant un affichage alternatif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exemple de nom pour le lien : “Contact”</t>
   </si>
 </sst>
 </file>
@@ -343,7 +388,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -491,16 +536,69 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E8" s="5"/>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E9" s="5"/>
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E10" s="5"/>
+      <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E11" s="5"/>
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E12" s="5"/>
@@ -1503,6 +1601,7 @@
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" display="https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB"/>
     <hyperlink ref="F7" r:id="rId2" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
+    <hyperlink ref="F9" r:id="rId3" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
optimisation index.html et report dans l'audit
</commit_message>
<xml_diff>
--- a/audit_seo.xlsx
+++ b/audit_seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -158,6 +158,115 @@
   </si>
   <si>
     <t xml:space="preserve">exemple de nom pour le lien : “Contact”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.69): description subjective du site dans une balise alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.87): insertion d’un segment de texte sous forme d’image au lieu d’intégrer le texte directement au code html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">une image étant plus volumineuse que du texte codé, cette pratique accentue la lenteur du site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coder le texte sous html au lieu d’intégrer des images ne contenant que du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer l’image du code html et la remplacer par du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sémentique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.110): présence d’une balise &lt;br&gt; inutile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la balise &lt;br&gt; permet un retour à la ligne, mais dans ce cas de figure elle est dispensable puisqu’elle se situe à la fin du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">éviter les structures dispensables pour faciliter la compréhension du site lors de sa lecture, et dans une plus moindre mesure réduire son poids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer cette balise</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(index.html l.127):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> insertion d’un segment de texte sous forme d’image au lieu d’intégrer le texte directement au code html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.141): présence d’une balise &lt;br&gt; inutile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.157): insertion d’un segment de texte sous forme d’image au lieu d’intégrer le texte directement au code html </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(index.html l.162): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">description subjective du site dans une balise alt</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">exemple de description : “Refonte d'un site web pour un journal local”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.171): description subjective du site dans une balise alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exemple de description : “Création d'un site web pour photographes”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.182): description subjective du site dans une balise alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exemple de description : “Création d'un site web pour voyageur”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.191): description subjective du site dans une balise alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exemple de description : “Création d'un site web pour agence de mariage”</t>
   </si>
 </sst>
 </file>
@@ -168,7 +277,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-2000]#,##0.00;[RED]\-[$$-2000]#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -226,6 +335,12 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -275,7 +390,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -304,7 +419,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -388,7 +511,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -601,24 +724,178 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E12" s="5"/>
+      <c r="A12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E13" s="5"/>
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E14" s="5"/>
+      <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D22" s="8"/>
+    </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1601,7 +1878,7 @@
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" display="https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB"/>
     <hyperlink ref="F7" r:id="rId2" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
-    <hyperlink ref="F9" r:id="rId3" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran"/>
+    <hyperlink ref="F9" r:id="rId3" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
correction liens css et java pour page2.html
</commit_message>
<xml_diff>
--- a/audit_seo.xlsx
+++ b/audit_seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Référence</t>
   </si>
   <si>
-    <t xml:space="preserve">(SEO ou accessiblité ?)</t>
+    <t xml:space="preserve">INDEX.HTML</t>
   </si>
   <si>
     <t xml:space="preserve">accessibilité</t>
@@ -268,6 +268,30 @@
   <si>
     <t xml:space="preserve">exemple de description : “Création d'un site web pour agence de mariage”</t>
   </si>
+  <si>
+    <t xml:space="preserve">PAGE2.HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(page2.html l.2): langue de la page index.html paramétrée sur “default”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(page2,html l.10 à l.20): erreur de cheminement pour les fichiers css et java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">du fait du mauvais cheminement du chargement des fichiers css et java, certaines mises en formes n’étaient pas fonctionnelles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vérifier que le cheminement est valide lorsqu’un lien est établi vers un document externe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corriger les liens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(page2.html l.22): meta title vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exemple de titre : “Contact”</t>
+  </si>
 </sst>
 </file>
 
@@ -277,7 +301,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-2000]#,##0.00;[RED]\-[$$-2000]#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -317,10 +341,11 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -340,6 +365,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -390,7 +423,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -428,6 +461,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -494,7 +531,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -508,10 +545,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -896,10 +933,62 @@
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D22" s="8"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1874,6 +1963,7 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" display="https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB"/>

</xml_diff>

<commit_message>
Ajout recommandations dans audit
</commit_message>
<xml_diff>
--- a/audit_seo.xlsx
+++ b/audit_seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -195,10 +195,9 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
-      <t xml:space="preserve">(index.html l.127):</t>
+      <t xml:space="preserve">(index.html l.127): insertion d’un segment de texte sous forme d’image au lieu d’intégrer le texte directement au code html</t>
     </r>
     <r>
       <rPr>
@@ -207,16 +206,6 @@
         <rFont val="Arial"/>
         <family val="0"/>
       </rPr>
-      <t xml:space="preserve"> insertion d’un segment de texte sous forme d’image au lieu d’intégrer le texte directement au code html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve"> </t>
     </r>
   </si>
@@ -227,25 +216,7 @@
     <t xml:space="preserve">(index.html l.157): insertion d’un segment de texte sous forme d’image au lieu d’intégrer le texte directement au code html </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(index.html l.162): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">description subjective du site dans une balise alt</t>
-    </r>
+    <t xml:space="preserve">(index.html l.162): description subjective du site dans une balise alt</t>
   </si>
   <si>
     <t xml:space="preserve">exemple de description : “Refonte d'un site web pour un journal local”</t>
@@ -275,7 +246,7 @@
     <t xml:space="preserve">(page2.html l.2): langue de la page index.html paramétrée sur “default”</t>
   </si>
   <si>
-    <t xml:space="preserve">(page2,html l.10 à l.20): erreur de cheminement pour les fichiers css et java</t>
+    <t xml:space="preserve">(page2.html l.10 à l.20): erreur de cheminement pour les fichiers css et java</t>
   </si>
   <si>
     <t xml:space="preserve">du fait du mauvais cheminement du chargement des fichiers css et java, certaines mises en formes n’étaient pas fonctionnelles</t>
@@ -291,6 +262,33 @@
   </si>
   <si>
     <t xml:space="preserve">exemple de titre : “Contact”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(page2.html l.34 à l.57): erreur de cheminement pour les fichiers css et java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reprise du menu de navigation de la page index.html corrigée, du fait de la présence des mêmes erreurs que constatées sur celle-ci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voir lignes 10 et 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STYLE.CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(style.css l.778): la couleur du texte est trop proche de la couleur de fond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tout le monde n’a pas la même vue, et les personnes malvoyantes ou daltoniennes peuvent ne pas voir le texte si le contraste entre la couleur du fond et de celui-ci n’est pas assez élevé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en cas de doute sur la visibilité </t>
+  </si>
+  <si>
+    <t xml:space="preserve">changer la couleur du texte (en blanc par exemple)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast</t>
   </si>
 </sst>
 </file>
@@ -301,13 +299,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-2000]#,##0.00;[RED]\-[$$-2000]#,##0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -330,7 +327,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -338,7 +334,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -352,30 +347,15 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color rgb="FFC9211E"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +366,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF77BC65"/>
+        <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
   </fills>
@@ -452,6 +438,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -460,11 +450,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -526,7 +512,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -548,7 +534,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -619,7 +605,7 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -648,10 +634,10 @@
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -668,7 +654,7 @@
       <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -688,7 +674,7 @@
       <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="7" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -708,7 +694,7 @@
       <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -725,7 +711,7 @@
       <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -753,7 +739,7 @@
       <c r="C11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -773,7 +759,7 @@
       <c r="D12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -790,7 +776,7 @@
       <c r="D13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -815,7 +801,7 @@
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -824,7 +810,7 @@
       <c r="D15" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -841,7 +827,7 @@
       <c r="D16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -858,7 +844,7 @@
       <c r="D17" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -866,7 +852,7 @@
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -875,7 +861,7 @@
       <c r="D18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="10" t="s">
         <v>60</v>
       </c>
     </row>
@@ -892,7 +878,7 @@
       <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="10" t="s">
         <v>62</v>
       </c>
     </row>
@@ -909,7 +895,7 @@
       <c r="D20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="10" t="s">
         <v>64</v>
       </c>
     </row>
@@ -926,7 +912,7 @@
       <c r="D21" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="10" t="s">
         <v>66</v>
       </c>
     </row>
@@ -934,7 +920,7 @@
       <c r="D22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="4" t="s">
         <v>67</v>
       </c>
     </row>
@@ -951,7 +937,7 @@
       <c r="D24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -968,7 +954,7 @@
       <c r="D25" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="5" t="s">
         <v>72</v>
       </c>
     </row>
@@ -985,14 +971,53 @@
       <c r="D26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1969,6 +1994,7 @@
     <hyperlink ref="F6" r:id="rId1" display="https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB"/>
     <hyperlink ref="F7" r:id="rId2" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
     <hyperlink ref="F9" r:id="rId3" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F30" r:id="rId4" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Déplacement des fichiers js à la fin du code html
</commit_message>
<xml_diff>
--- a/audit_seo.xlsx
+++ b/audit_seo.xlsx
@@ -196,6 +196,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(index.html l.127): insertion d’un segment de texte sous forme d’image au lieu d’intégrer le texte directement au code html</t>
     </r>
@@ -205,6 +206,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -305,6 +307,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -327,6 +330,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -334,6 +338,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -341,18 +346,21 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -534,7 +542,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -608,6 +616,9 @@
       <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="G3" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -640,6 +651,9 @@
       <c r="E5" s="7" t="s">
         <v>19</v>
       </c>
+      <c r="G5" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -660,6 +674,9 @@
       <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="G6" s="1" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -680,6 +697,9 @@
       <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="G7" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -697,6 +717,9 @@
       <c r="E8" s="7" t="s">
         <v>34</v>
       </c>
+      <c r="G8" s="1" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -717,6 +740,9 @@
       <c r="F9" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="G9" s="1" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -742,8 +768,11 @@
       <c r="D11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="7" t="s">
         <v>45</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -762,6 +791,9 @@
       <c r="E12" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="G12" s="1" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -779,6 +811,9 @@
       <c r="E13" s="7" t="s">
         <v>50</v>
       </c>
+      <c r="G13" s="1" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -813,6 +848,9 @@
       <c r="E15" s="7" t="s">
         <v>50</v>
       </c>
+      <c r="G15" s="1" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -847,6 +885,9 @@
       <c r="E17" s="7" t="s">
         <v>50</v>
       </c>
+      <c r="G17" s="1" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -864,6 +905,9 @@
       <c r="E18" s="10" t="s">
         <v>60</v>
       </c>
+      <c r="G18" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -881,6 +925,9 @@
       <c r="E19" s="10" t="s">
         <v>62</v>
       </c>
+      <c r="G19" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -898,6 +945,9 @@
       <c r="E20" s="10" t="s">
         <v>64</v>
       </c>
+      <c r="G20" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -915,6 +965,9 @@
       <c r="E21" s="10" t="s">
         <v>66</v>
       </c>
+      <c r="G21" s="1" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D22" s="8"/>
@@ -940,6 +993,9 @@
       <c r="E24" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="G24" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
@@ -973,6 +1029,9 @@
       </c>
       <c r="E26" s="7" t="s">
         <v>74</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1016,6 +1075,9 @@
       </c>
       <c r="F30" s="1" t="s">
         <v>83</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Compression des images du site
</commit_message>
<xml_diff>
--- a/audit_seo.xlsx
+++ b/audit_seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -242,6 +242,36 @@
     <t xml:space="preserve">exemple de description : “Création d'un site web pour agence de mariage”</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(index.html l.248): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">texte “caché” comprenant des mots clés pour tromper les algorithmes de Google lors de la lecture de la page web pour son référencement</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">(index.html l.250 à l.288): footer contenant beaucoup de liens pour tenter d’améliorer le référencement du site en trompant les algorithmes des moteurs de recherche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n’utiliser que des liens pertinents dans le footer, et garder une présentation épurée pour une meilleure expérience utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer ces liens</t>
+  </si>
+  <si>
     <t xml:space="preserve">PAGE2.HTML</t>
   </si>
   <si>
@@ -301,7 +331,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-2000]#,##0.00;[RED]\-[$$-2000]#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -362,6 +392,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -417,7 +453,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -459,6 +495,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -539,10 +583,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -970,96 +1014,113 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D22" s="8"/>
+      <c r="A22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>67</v>
+      <c r="A23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="B27" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="1" t="n">
+      <c r="G27" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="B28" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="8" t="s">
+      <c r="B29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" s="1" t="n">
+      <c r="E29" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="1" t="n">
         <v>4</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>79</v>
@@ -1070,19 +1131,39 @@
       <c r="D30" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="1" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G30" s="1" t="n">
+      <c r="C33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="1" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2051,12 +2132,15 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" display="https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB"/>
     <hyperlink ref="F7" r:id="rId2" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
     <hyperlink ref="F9" r:id="rId3" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
-    <hyperlink ref="F30" r:id="rId4" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
+    <hyperlink ref="F33" r:id="rId4" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
mise à jour audit et comparaison performances
</commit_message>
<xml_diff>
--- a/audit_seo.xlsx
+++ b/audit_seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="97">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -52,48 +52,57 @@
     <t xml:space="preserve">peut occasionner des difficultés de lectures pour les utilisateurs de lecteurs d’écran</t>
   </si>
   <si>
-    <t xml:space="preserve">paramétrer la langue en fonction de celle utilisée par la page (spécifier pour des passages qui seraient dans une autre langue si besoin)</t>
-  </si>
-  <si>
     <t xml:space="preserve">régler la langue sur “fr”</t>
   </si>
   <si>
+    <t xml:space="preserve">X (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/International/questions/qa-html-language-declarations.fr</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO</t>
   </si>
   <si>
     <t xml:space="preserve">(index.html l.5): utilisation multiple du mot clé “agence design”</t>
   </si>
   <si>
-    <t xml:space="preserve">En plus de créer une répétition inutile, il est préférable d’éviter les pratiques pouvant être interprétées comme un abus de fonctionnement des algorithmes de recherche</t>
+    <t xml:space="preserve">En plus de créer une répétition inutile, il est préférable d’éviter les pratiques pouvant être interprétées comme un abus de fonctionnement des algorithmes de recherche, bien que ceux-ci l’ignorent de plus en plus</t>
   </si>
   <si>
     <t xml:space="preserve">choisir des mots clés pertinents en favorisant l’approche longue traîne à l’approche courte traîne</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.definitions-seo.com/definition-de-balise-meta-keywords/#:~:text=La%20balise%20meta%20Keywords%20est,plus%20aucun%20poids%20en%20SEO%E2%80%A6</t>
+  </si>
+  <si>
     <t xml:space="preserve">(index.html l.5): utilisation du mot clé “agence design Paris” alors que l’agence est basée à Lyon</t>
   </si>
   <si>
     <t xml:space="preserve">Indiquer une autre localisation que celle de l’enseigne de l’agence induira les visiteurs potentiels en erreur leurs de leur recherche, en plus de créer une plus grande concurrence dans les résultats de recherche (Paris vs Lyon)</t>
   </si>
   <si>
-    <t xml:space="preserve">Les mots clés locaux doivent désigner la même localisation que celle indiquée sur le site web et qui reflète la position géographique réelle de l’enseigne physique de l’agence</t>
-  </si>
-  <si>
     <t xml:space="preserve">remplacer “Paris” par “Lyon”</t>
   </si>
   <si>
+    <t xml:space="preserve">X (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://optimiz.me/le-referencement-local/</t>
+  </si>
+  <si>
     <t xml:space="preserve">(index.html l.6): meta description vide</t>
   </si>
   <si>
     <t xml:space="preserve">la meta description représente le texte qui sera affiché sous le titre et url du site dans les résultats de recherche, et est un facteur important d’attraction pour les visiteurs potentiels</t>
   </si>
   <si>
-    <t xml:space="preserve">utiliser une description pertinente (incluant les mots clés du site) et consise (moins de 140-160 caractères) tout en restant attirante pour les visiteurs potentiels</t>
-  </si>
-  <si>
     <t xml:space="preserve">exemple de description : “La Chouette agence web design à Lyon : réalisez votre projet web grâce à notre expertise”</t>
   </si>
   <si>
+    <t xml:space="preserve">X (3)</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB</t>
   </si>
   <si>
@@ -106,12 +115,12 @@
     <t xml:space="preserve">la meta titre est ce qui sera affiché en premier lors de l’apparition du site web dans les résultats de recherche et se doit donc d’être attractif</t>
   </si>
   <si>
-    <t xml:space="preserve">utiliser un titre concis et reprenant des mots clés de manière pertinente et naturelle</t>
-  </si>
-  <si>
     <t xml:space="preserve">exemple de titre : “La Chouette agence | Experts web design à Lyon”</t>
   </si>
   <si>
+    <t xml:space="preserve">x (4)</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq</t>
   </si>
   <si>
@@ -121,45 +130,54 @@
     <t xml:space="preserve">ce genre de pratique, en plus d’être de mieux en mieux détecté par les algorithmes de Google, peut amener à une pénalisation du site web dans son référencement</t>
   </si>
   <si>
-    <t xml:space="preserve">n’utiliser des mots clés que dans des contextes pertinents et proscrire ce genre de pratique</t>
-  </si>
-  <si>
     <t xml:space="preserve">supprimer ces balises</t>
   </si>
   <si>
+    <t xml:space="preserve">X (5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr</t>
+  </si>
+  <si>
     <t xml:space="preserve">(index.html l.41): description subjective du site dans une balise alt</t>
   </si>
   <si>
     <t xml:space="preserve">les balises alt servent non seulement à décrire un élément visuel, mais sont également utilisées pour vérifier la pertinence d’un contenu par les moteurs de recherche</t>
   </si>
   <si>
-    <t xml:space="preserve">se contenter d’utiliser les balises alt pour fournir de courtes descriptions objectives des éléments relatifs à celles-ci</t>
-  </si>
-  <si>
     <t xml:space="preserve">exemple de description : “logo La Chouette agence”</t>
   </si>
   <si>
+    <t xml:space="preserve">X (6)</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran.</t>
   </si>
   <si>
-    <t xml:space="preserve">???SEO???</t>
+    <t xml:space="preserve">sémentique</t>
   </si>
   <si>
     <t xml:space="preserve">(index.html l.52 et l.53): balise &lt;li&gt;&lt;/li&gt; vide</t>
   </si>
   <si>
+    <t xml:space="preserve">bien que cela ne constitue pas une erreur en soit et par soucis de lisibilité du code html, il est envisageable de supprimer ces balises vides</t>
+  </si>
+  <si>
     <t xml:space="preserve">(index.html l.55): nom affiché sur le site pour la redirection vers page2.html (“page2 &amp;gt;”)</t>
   </si>
   <si>
     <t xml:space="preserve">en plus de la faute de frappe pouvait donner une image amateure du site et le décrédibiliser auprès des visiteurs, nommer un lien “page2” ne permet pas de savoir vers quoi celui-ci redirige</t>
   </si>
   <si>
-    <t xml:space="preserve">les liens affichés sur le site devraient refléter clairement le type de contenu vers lequels ils redirigent afin de faciliter la navigation sur le site web, d’autant plus pour les personnes utilisant un affichage alternatif</t>
-  </si>
-  <si>
     <t xml:space="preserve">exemple de nom pour le lien : “Contact”</t>
   </si>
   <si>
+    <t xml:space="preserve">X (7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://audreytips.com/orthographe-contenus-web/</t>
+  </si>
+  <si>
     <t xml:space="preserve">(index.html l.69): description subjective du site dans une balise alt</t>
   </si>
   <si>
@@ -169,22 +187,16 @@
     <t xml:space="preserve">une image étant plus volumineuse que du texte codé, cette pratique accentue la lenteur du site</t>
   </si>
   <si>
-    <t xml:space="preserve">coder le texte sous html au lieu d’intégrer des images ne contenant que du texte</t>
-  </si>
-  <si>
     <t xml:space="preserve">supprimer l’image du code html et la remplacer par du texte</t>
   </si>
   <si>
-    <t xml:space="preserve">sémentique</t>
+    <t xml:space="preserve">X (8)</t>
   </si>
   <si>
     <t xml:space="preserve">(index.html l.110): présence d’une balise &lt;br&gt; inutile</t>
   </si>
   <si>
     <t xml:space="preserve">la balise &lt;br&gt; permet un retour à la ligne, mais dans ce cas de figure elle est dispensable puisqu’elle se situe à la fin du texte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">éviter les structures dispensables pour faciliter la compréhension du site lors de sa lecture, et dans une plus moindre mesure réduire son poids</t>
   </si>
   <si>
     <t xml:space="preserve">supprimer cette balise</t>
@@ -242,33 +254,12 @@
     <t xml:space="preserve">exemple de description : “Création d'un site web pour agence de mariage”</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(index.html l.248): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">texte “caché” comprenant des mots clés pour tromper les algorithmes de Google lors de la lecture de la page web pour son référencement</t>
-    </r>
+    <t xml:space="preserve">(index.html l.248): texte “caché” comprenant des mots clés pour tromper les algorithmes de Google lors de la lecture de la page web pour son référencement</t>
   </si>
   <si>
     <t xml:space="preserve">(index.html l.250 à l.288): footer contenant beaucoup de liens pour tenter d’améliorer le référencement du site en trompant les algorithmes des moteurs de recherche</t>
   </si>
   <si>
-    <t xml:space="preserve">n’utiliser que des liens pertinents dans le footer, et garder une présentation épurée pour une meilleure expérience utilisateur</t>
-  </si>
-  <si>
     <t xml:space="preserve">supprimer ces liens</t>
   </si>
   <si>
@@ -284,9 +275,6 @@
     <t xml:space="preserve">du fait du mauvais cheminement du chargement des fichiers css et java, certaines mises en formes n’étaient pas fonctionnelles</t>
   </si>
   <si>
-    <t xml:space="preserve">vérifier que le cheminement est valide lorsqu’un lien est établi vers un document externe</t>
-  </si>
-  <si>
     <t xml:space="preserve">corriger les liens</t>
   </si>
   <si>
@@ -296,6 +284,9 @@
     <t xml:space="preserve">exemple de titre : “Contact”</t>
   </si>
   <si>
+    <t xml:space="preserve">X (4)</t>
+  </si>
+  <si>
     <t xml:space="preserve">(page2.html l.34 à l.57): erreur de cheminement pour les fichiers css et java</t>
   </si>
   <si>
@@ -314,13 +305,31 @@
     <t xml:space="preserve">Tout le monde n’a pas la même vue, et les personnes malvoyantes ou daltoniennes peuvent ne pas voir le texte si le contraste entre la couleur du fond et de celui-ci n’est pas assez élevé</t>
   </si>
   <si>
-    <t xml:space="preserve">en cas de doute sur la visibilité </t>
-  </si>
-  <si>
     <t xml:space="preserve">changer la couleur du texte (en blanc par exemple)</t>
   </si>
   <si>
+    <t xml:space="preserve">X (9)</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGES UTILISÉES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le format (et donc la taille) des images utilisées est plus volumineuse que nécessaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il est préférable d’éviter certains formats d’image comme .jpeg ou .bmp lorsque cela est possible, car ces formats sont lourds et ralentissent fortement la vitesse du site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choisir le format d’image le plus adapté à chaque besoin et compresser celles-ci / convertir les images vers un format plus léger comme le format .webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X (10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.anthedesign.fr/creation-de-sites-internet/format-webp/</t>
   </si>
 </sst>
 </file>
@@ -331,7 +340,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-2000]#,##0.00;[RED]\-[$$-2000]#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -388,6 +397,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -398,8 +413,15 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,12 +432,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF993366"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF77BC65"/>
-        <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
   </fills>
@@ -453,13 +469,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -475,18 +495,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -494,7 +506,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -502,7 +518,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,7 +588,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF77BC65"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -586,559 +610,537 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="1" width="10.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="1" width="11.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <v>1</v>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>48</v>
+        <v>13</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>7</v>
+        <v>55</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>48</v>
+        <v>13</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>7</v>
+        <v>55</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>8</v>
+      <c r="B18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>61</v>
+      <c r="B19" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="1" t="n">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>8</v>
+      <c r="B20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E22" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>5</v>
+      <c r="F22" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>70</v>
-      </c>
+      <c r="A23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D24" s="8"/>
+      <c r="D24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D25" s="8"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>71</v>
+      <c r="A26" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="B27" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="1" t="n">
-        <v>1</v>
+      <c r="F27" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>74</v>
+      <c r="A28" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>76</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>27</v>
+      <c r="A29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="1" t="n">
-        <v>4</v>
+        <v>80</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>82</v>
+      <c r="A32" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1146,27 +1148,47 @@
         <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>9</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2137,10 +2159,24 @@
     <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" display="https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB"/>
-    <hyperlink ref="F7" r:id="rId2" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
-    <hyperlink ref="F9" r:id="rId3" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
-    <hyperlink ref="F33" r:id="rId4" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
+    <hyperlink ref="F3" r:id="rId1" display="https://www.w3.org/International/questions/qa-html-language-declarations.fr"/>
+    <hyperlink ref="F4" r:id="rId2" location=":~:text=La%20balise%20meta%20Keywords%20est,plus%20aucun%20poids%20en%20SEO…" display="https://www.definitions-seo.com/definition-de-balise-meta-keywords/#:~:text=La%20balise%20meta%20Keywords%20est,plus%20aucun%20poids%20en%20SEO%E2%80%A6"/>
+    <hyperlink ref="F5" r:id="rId3" display="https://optimiz.me/le-referencement-local/"/>
+    <hyperlink ref="F6" r:id="rId4" display="https://fr.semrush.com/blog/basiques-seo-meta-description/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_FR&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=486541998946&amp;kwid=dsa-1100351993444&amp;cmpid=11849486850&amp;agpid=113156847337&amp;BU=Core&amp;extid=152584053920&amp;adpos=&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eev92Q2ZeZK4yA-iSkFkYEiwxEgfzUr5Uacz9ny1okQI7IidBZNVZGYaAuEbEALw_wcB"/>
+    <hyperlink ref="F7" r:id="rId5" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
+    <hyperlink ref="F8" r:id="rId6" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
+    <hyperlink ref="F9" r:id="rId7" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F11" r:id="rId8" display="https://audreytips.com/orthographe-contenus-web/"/>
+    <hyperlink ref="F12" r:id="rId9" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F18" r:id="rId10" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F19" r:id="rId11" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F20" r:id="rId12" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F21" r:id="rId13" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F22" r:id="rId14" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
+    <hyperlink ref="F27" r:id="rId15" display="https://www.w3.org/International/questions/qa-html-language-declarations.fr"/>
+    <hyperlink ref="F29" r:id="rId16" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
+    <hyperlink ref="F33" r:id="rId17" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
+    <hyperlink ref="F36" r:id="rId18" display="https://www.anthedesign.fr/creation-de-sites-internet/format-webp/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
correction audit seo et form page contact
</commit_message>
<xml_diff>
--- a/audit_seo.xlsx
+++ b/audit_seo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="88">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -154,15 +154,6 @@
     <t xml:space="preserve">https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran.</t>
   </si>
   <si>
-    <t xml:space="preserve">sémentique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(index.html l.52 et l.53): balise &lt;li&gt;&lt;/li&gt; vide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bien que cela ne constitue pas une erreur en soit et par soucis de lisibilité du code html, il est envisageable de supprimer ces balises vides</t>
-  </si>
-  <si>
     <t xml:space="preserve">(index.html l.55): nom affiché sur le site pour la redirection vers page2.html (“page2 &amp;gt;”)</t>
   </si>
   <si>
@@ -193,13 +184,7 @@
     <t xml:space="preserve">X (8)</t>
   </si>
   <si>
-    <t xml:space="preserve">(index.html l.110): présence d’une balise &lt;br&gt; inutile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">la balise &lt;br&gt; permet un retour à la ligne, mais dans ce cas de figure elle est dispensable puisqu’elle se situe à la fin du texte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supprimer cette balise</t>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist</t>
   </si>
   <si>
     <r>
@@ -224,9 +209,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">(index.html l.141): présence d’une balise &lt;br&gt; inutile</t>
-  </si>
-  <si>
     <t xml:space="preserve">(index.html l.157): insertion d’un segment de texte sous forme d’image au lieu d’intégrer le texte directement au code html </t>
   </si>
   <si>
@@ -267,15 +249,6 @@
   </si>
   <si>
     <t xml:space="preserve">(page2.html l.2): langue de la page index.html paramétrée sur “default”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(page2.html l.10 à l.20): erreur de cheminement pour les fichiers css et java</t>
-  </si>
-  <si>
-    <t xml:space="preserve">du fait du mauvais cheminement du chargement des fichiers css et java, certaines mises en formes n’étaient pas fonctionnelles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">corriger les liens</t>
   </si>
   <si>
     <t xml:space="preserve">(page2.html l.22): meta title vide</t>
@@ -340,7 +313,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-2000]#,##0.00;[RED]\-[$$-2000]#,##0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -397,28 +370,9 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color rgb="FFC9211E"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -469,7 +423,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -502,32 +456,20 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -607,10 +549,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -779,7 +721,7 @@
       <c r="D8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -799,7 +741,7 @@
       <c r="D9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -808,57 +750,62 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>48</v>
+      <c r="A11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="C12" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="D12" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>42</v>
+      <c r="E12" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -866,96 +813,115 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="F13" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="6"/>
+        <v>52</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>56</v>
+        <v>7</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>56</v>
+      <c r="E17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -963,232 +929,161 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="B24" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
+      <c r="B29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="C32" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
+      <c r="D32" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2153,10 +2048,10 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://www.w3.org/International/questions/qa-html-language-declarations.fr"/>
@@ -2166,17 +2061,20 @@
     <hyperlink ref="F7" r:id="rId5" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
     <hyperlink ref="F8" r:id="rId6" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
     <hyperlink ref="F9" r:id="rId7" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
-    <hyperlink ref="F11" r:id="rId8" display="https://audreytips.com/orthographe-contenus-web/"/>
-    <hyperlink ref="F12" r:id="rId9" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
-    <hyperlink ref="F18" r:id="rId10" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
-    <hyperlink ref="F19" r:id="rId11" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
-    <hyperlink ref="F20" r:id="rId12" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
-    <hyperlink ref="F21" r:id="rId13" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
-    <hyperlink ref="F22" r:id="rId14" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
-    <hyperlink ref="F27" r:id="rId15" display="https://www.w3.org/International/questions/qa-html-language-declarations.fr"/>
-    <hyperlink ref="F29" r:id="rId16" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
-    <hyperlink ref="F33" r:id="rId17" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
-    <hyperlink ref="F36" r:id="rId18" display="https://www.anthedesign.fr/creation-de-sites-internet/format-webp/"/>
+    <hyperlink ref="F10" r:id="rId8" display="https://audreytips.com/orthographe-contenus-web/"/>
+    <hyperlink ref="F11" r:id="rId9" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F12" r:id="rId10" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist"/>
+    <hyperlink ref="F13" r:id="rId11" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist"/>
+    <hyperlink ref="F14" r:id="rId12" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist"/>
+    <hyperlink ref="F15" r:id="rId13" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F16" r:id="rId14" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F17" r:id="rId15" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F18" r:id="rId16" location=":~:text=La%20balise%20ALT%2C%20également%20connue,apparaît%20pas%20à%20l'écran" display="https://www.atinternet.com/glossaire/balise-alt/#:~:text=La%20balise%20ALT%2C%20%C3%A9galement%20connue,appara%C3%AEt%20pas%20%C3%A0%20l'%C3%A9cran."/>
+    <hyperlink ref="F19" r:id="rId17" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
+    <hyperlink ref="F24" r:id="rId18" display="https://www.w3.org/International/questions/qa-html-language-declarations.fr"/>
+    <hyperlink ref="F25" r:id="rId19" display="https://university.webflow.com/lesson/seo-title-meta-description?utm_source=google&amp;utm_medium=search&amp;utm_campaign=general-paid-workhorse&amp;utm_term=keyword-targeting&amp;utm_content=dynamic-search-ads-webflow-university-t1&amp;gclid=Cj0KCQjw7MGJBhD-ARIsAMZ0eevWyJeq"/>
+    <hyperlink ref="F29" r:id="rId20" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast"/>
+    <hyperlink ref="F32" r:id="rId21" display="https://www.anthedesign.fr/creation-de-sites-internet/format-webp/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>